<commit_message>
MA_09_02_CO y MA_05_03_CO. Seguimiento.
</commit_message>
<xml_diff>
--- a/seguimiento/Grado05.xlsx
+++ b/seguimiento/Grado05.xlsx
@@ -840,7 +840,7 @@
   <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,10 +990,18 @@
       <c r="A8" s="29">
         <v>3</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="B8" s="4">
+        <v>42102</v>
+      </c>
+      <c r="C8" s="4">
+        <v>42102</v>
+      </c>
+      <c r="D8" s="4">
+        <v>42104</v>
+      </c>
+      <c r="E8" s="4">
+        <v>42102</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
@@ -1227,7 +1235,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
       <formula1>"3,4,5,6,7,8,9,10,11"</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:E21 G6:G21 K6:K21">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K21 G6:G21 B6:E21">
       <formula1>42005</formula1>
       <formula2>42461</formula2>
     </dataValidation>

</xml_diff>